<commit_message>
clase de Excel para generación de archivos.
clase de estilos para el archivo de Excel (títulos y detalle).
</commit_message>
<xml_diff>
--- a/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/bosch_spread.xlsx
+++ b/01-CodigoFuente/main/Spooler/main/main/bin/Debug/net8.0/bosch_spread.xlsx
@@ -6,8 +6,8 @@
     <x:workbookView activeTab="1"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Exportación" sheetId="1" r:id="Re28df7aa78bd43da"/>
-    <x:sheet name="Importación" sheetId="2" r:id="Rfbecbc32ad3c4419"/>
+    <x:sheet name="Exportación" sheetId="1" r:id="R81a601a5241b4fb5"/>
+    <x:sheet name="Importación" sheetId="2" r:id="Ra4158220e2534bdb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -370,7 +370,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="4">
+  <x:fonts count="3">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -380,12 +380,7 @@
     <x:font>
       <x:b/>
       <x:sz val="8"/>
-      <x:name val="Arial"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-      <x:sz val="8"/>
-      <x:color theme="1"/>
+      <x:color rgb="FF000000"/>
       <x:name val="Arial"/>
     </x:font>
     <x:font>
@@ -395,12 +390,18 @@
       <x:name val="Arial"/>
     </x:font>
   </x:fonts>
-  <x:fills count="3">
+  <x:fills count="4">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFFFF"/>
+        <x:bgColor rgb="FF000000"/>
+      </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
@@ -423,17 +424,17 @@
   </x:cellStyleXfs>
   <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <x:alignment shrinkToFit="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <x:alignment shrinkToFit="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">

</xml_diff>